<commit_message>
updated import spreadhseet with errors for presentation
</commit_message>
<xml_diff>
--- a/import_files/giftdriver_drive2ee (2013 Annual Gift Drive ).xlsx
+++ b/import_files/giftdriver_drive2ee (2013 Annual Gift Drive ).xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="175">
   <si>
     <t>first_name</t>
   </si>
@@ -193,9 +193,6 @@
     <t>hoodie</t>
   </si>
   <si>
-    <t>Philip</t>
-  </si>
-  <si>
     <t>xl</t>
   </si>
   <si>
@@ -307,9 +304,6 @@
     <t>shirt</t>
   </si>
   <si>
-    <t>Isabella</t>
-  </si>
-  <si>
     <t>Isabella is a smart cookie who loves finger painting, dogs, and Teletubbies.</t>
   </si>
   <si>
@@ -470,9 +464,6 @@
   </si>
   <si>
     <t>bluray player</t>
-  </si>
-  <si>
-    <t>Jasmin</t>
   </si>
   <si>
     <t>Jasmin is working on getting her associate's degree part time, and spends every free moment she can with Samuel and Mateo. She loves to cook and listen to opera.</t>
@@ -968,20 +959,14 @@
       <c s="1" r="P7"/>
     </row>
     <row r="8">
-      <c t="s" s="1" r="A8">
-        <v>60</v>
-      </c>
+      <c s="1" r="A8"/>
       <c s="1" r="B8">
         <v>30</v>
       </c>
-      <c t="s" s="1" r="C8">
-        <v>29</v>
-      </c>
-      <c s="1" r="D8">
-        <v>32</v>
-      </c>
+      <c s="1" r="C8"/>
+      <c s="1" r="D8"/>
       <c t="s" s="1" r="E8">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c t="s" s="1" r="F8">
         <v>31</v>
@@ -990,28 +975,28 @@
         <v>12</v>
       </c>
       <c t="s" s="1" r="H8">
+        <v>61</v>
+      </c>
+      <c t="s" s="1" r="I8">
         <v>62</v>
       </c>
-      <c t="s" s="1" r="I8">
+      <c t="s" s="1" r="J8">
+        <v>21</v>
+      </c>
+      <c t="s" s="1" r="K8">
         <v>63</v>
       </c>
-      <c t="s" s="1" r="J8">
-        <v>21</v>
-      </c>
-      <c t="s" s="1" r="K8">
+      <c t="s" s="1" r="L8">
         <v>64</v>
       </c>
-      <c t="s" s="1" r="L8">
+      <c t="s" s="1" r="M8">
         <v>65</v>
-      </c>
-      <c t="s" s="1" r="M8">
-        <v>66</v>
       </c>
       <c t="s" s="1" r="N8">
         <v>26</v>
       </c>
       <c t="s" s="1" r="O8">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c t="s" s="1" r="P8">
         <v>58</v>
@@ -1023,7 +1008,7 @@
     </row>
     <row r="9">
       <c t="s" s="1" r="A9">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c s="1" r="B9">
         <v>26</v>
@@ -1044,10 +1029,10 @@
         <v>5</v>
       </c>
       <c t="s" s="1" r="H9">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c t="s" s="1" r="I9">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c t="s" s="1" r="J9">
         <v>21</v>
@@ -1073,7 +1058,7 @@
     </row>
     <row r="10">
       <c t="s" s="1" r="A10">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c s="1" r="B10">
         <v>5</v>
@@ -1094,10 +1079,10 @@
         <v>2</v>
       </c>
       <c t="s" s="1" r="H10">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c t="s" s="1" r="I10">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c t="s" s="1" r="J10">
         <v>21</v>
@@ -1106,7 +1091,7 @@
         <v>34</v>
       </c>
       <c t="s" s="1" r="L10">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c t="s" s="1" r="M10">
         <v>58</v>
@@ -1123,7 +1108,7 @@
     </row>
     <row r="11">
       <c t="s" s="1" r="A11">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c s="1" r="B11">
         <v>9</v>
@@ -1144,10 +1129,10 @@
         <v>4</v>
       </c>
       <c t="s" s="1" r="H11">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c t="s" s="1" r="I11">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c t="s" s="1" r="J11">
         <v>21</v>
@@ -1162,10 +1147,10 @@
         <v>25</v>
       </c>
       <c t="s" s="1" r="N11">
+        <v>74</v>
+      </c>
+      <c t="s" s="1" r="O11">
         <v>75</v>
-      </c>
-      <c t="s" s="1" r="O11">
-        <v>76</v>
       </c>
       <c s="1" r="P11"/>
       <c s="1" r="Q11"/>
@@ -1175,7 +1160,7 @@
     </row>
     <row r="12">
       <c t="s" s="1" r="A12">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c s="1" r="B12">
         <v>1</v>
@@ -1184,37 +1169,37 @@
         <v>17</v>
       </c>
       <c t="s" s="1" r="D12">
+        <v>77</v>
+      </c>
+      <c t="s" s="1" r="E12">
+        <v>77</v>
+      </c>
+      <c t="s" s="1" r="F12">
+        <v>77</v>
+      </c>
+      <c t="s" s="1" r="G12">
+        <v>77</v>
+      </c>
+      <c t="s" s="1" r="H12">
         <v>78</v>
       </c>
-      <c t="s" s="1" r="E12">
-        <v>78</v>
-      </c>
-      <c t="s" s="1" r="F12">
-        <v>78</v>
-      </c>
-      <c t="s" s="1" r="G12">
-        <v>78</v>
-      </c>
-      <c t="s" s="1" r="H12">
+      <c t="s" s="1" r="I12">
+        <v>62</v>
+      </c>
+      <c t="s" s="1" r="J12">
+        <v>21</v>
+      </c>
+      <c t="s" s="1" r="K12">
         <v>79</v>
       </c>
-      <c t="s" s="1" r="I12">
-        <v>63</v>
-      </c>
-      <c t="s" s="1" r="J12">
-        <v>21</v>
-      </c>
-      <c t="s" s="1" r="K12">
+      <c t="s" s="1" r="L12">
         <v>80</v>
       </c>
-      <c t="s" s="1" r="L12">
+      <c t="s" s="1" r="M12">
         <v>81</v>
       </c>
-      <c t="s" s="1" r="M12">
+      <c t="s" s="1" r="N12">
         <v>82</v>
-      </c>
-      <c t="s" s="1" r="N12">
-        <v>83</v>
       </c>
       <c s="1" r="O12"/>
       <c s="1" r="P12"/>
@@ -1225,7 +1210,7 @@
     </row>
     <row r="13">
       <c t="s" s="1" r="A13">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c s="1" r="B13">
         <v>35</v>
@@ -1233,9 +1218,7 @@
       <c t="s" s="1" r="C13">
         <v>29</v>
       </c>
-      <c s="1" r="D13">
-        <v>36</v>
-      </c>
+      <c s="1" r="D13"/>
       <c t="s" s="1" r="E13">
         <v>44</v>
       </c>
@@ -1246,41 +1229,39 @@
         <v>12</v>
       </c>
       <c t="s" s="1" r="H13">
+        <v>84</v>
+      </c>
+      <c t="s" s="1" r="I13">
         <v>85</v>
       </c>
-      <c t="s" s="1" r="I13">
+      <c t="s" s="1" r="J13">
+        <v>21</v>
+      </c>
+      <c t="s" s="1" r="K13">
         <v>86</v>
       </c>
-      <c t="s" s="1" r="J13">
-        <v>21</v>
-      </c>
-      <c t="s" s="1" r="K13">
+      <c t="s" s="1" r="L13">
         <v>87</v>
-      </c>
-      <c t="s" s="1" r="L13">
-        <v>88</v>
       </c>
       <c t="s" s="1" r="M13">
         <v>52</v>
       </c>
       <c t="s" s="1" r="N13">
+        <v>88</v>
+      </c>
+      <c t="s" s="1" r="O13">
         <v>89</v>
-      </c>
-      <c t="s" s="1" r="O13">
-        <v>90</v>
       </c>
       <c s="1" r="P13"/>
     </row>
     <row r="14">
       <c t="s" s="1" r="A14">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c s="1" r="B14">
         <v>25</v>
       </c>
-      <c t="s" s="1" r="C14">
-        <v>17</v>
-      </c>
+      <c s="1" r="C14"/>
       <c s="1" r="D14">
         <v>8</v>
       </c>
@@ -1294,10 +1275,10 @@
         <v>6</v>
       </c>
       <c t="s" s="1" r="H14">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c t="s" s="1" r="I14">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c t="s" s="1" r="J14">
         <v>21</v>
@@ -1306,22 +1287,22 @@
         <v>25</v>
       </c>
       <c t="s" s="1" r="L14">
+        <v>92</v>
+      </c>
+      <c t="s" s="1" r="M14">
         <v>93</v>
-      </c>
-      <c t="s" s="1" r="M14">
-        <v>94</v>
       </c>
       <c t="s" s="1" r="N14">
         <v>42</v>
       </c>
       <c t="s" s="1" r="O14">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c s="1" r="P14"/>
     </row>
     <row r="15">
       <c t="s" s="1" r="A15">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c s="1" r="B15">
         <v>10</v>
@@ -1342,10 +1323,10 @@
         <v>5</v>
       </c>
       <c t="s" s="1" r="H15">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c t="s" s="1" r="I15">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c t="s" s="1" r="J15">
         <v>21</v>
@@ -1354,21 +1335,19 @@
         <v>42</v>
       </c>
       <c t="s" s="1" r="L15">
+        <v>95</v>
+      </c>
+      <c t="s" s="1" r="M15">
         <v>96</v>
       </c>
-      <c t="s" s="1" r="M15">
-        <v>97</v>
-      </c>
       <c t="s" s="1" r="N15">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c s="1" r="O15"/>
       <c s="1" r="P15"/>
     </row>
     <row r="16">
-      <c t="s" s="1" r="A16">
-        <v>98</v>
-      </c>
+      <c s="1" r="A16"/>
       <c s="1" r="B16">
         <v>2</v>
       </c>
@@ -1388,10 +1367,10 @@
         <v>2</v>
       </c>
       <c t="s" s="1" r="H16">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c t="s" s="1" r="I16">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c t="s" s="1" r="J16">
         <v>21</v>
@@ -1415,7 +1394,7 @@
     </row>
     <row r="17">
       <c t="s" s="1" r="A17">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c s="1" r="B17">
         <v>25</v>
@@ -1436,22 +1415,22 @@
         <v>6</v>
       </c>
       <c t="s" s="1" r="H17">
+        <v>99</v>
+      </c>
+      <c t="s" s="1" r="I17">
+        <v>100</v>
+      </c>
+      <c t="s" s="1" r="J17">
+        <v>21</v>
+      </c>
+      <c t="s" s="1" r="K17">
         <v>101</v>
       </c>
-      <c t="s" s="1" r="I17">
+      <c t="s" s="1" r="L17">
         <v>102</v>
       </c>
-      <c t="s" s="1" r="J17">
-        <v>21</v>
-      </c>
-      <c t="s" s="1" r="K17">
-        <v>103</v>
-      </c>
-      <c t="s" s="1" r="L17">
-        <v>104</v>
-      </c>
       <c t="s" s="1" r="M17">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c t="s" s="1" r="N17">
         <v>25</v>
@@ -1460,7 +1439,7 @@
         <v>24</v>
       </c>
       <c t="s" s="1" r="P17">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c s="1" r="Q17"/>
       <c s="1" r="R17"/>
@@ -1469,7 +1448,7 @@
     </row>
     <row r="18">
       <c t="s" s="1" r="A18">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c s="1" r="B18">
         <v>3</v>
@@ -1490,10 +1469,10 @@
         <v>1</v>
       </c>
       <c t="s" s="1" r="H18">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c t="s" s="1" r="I18">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c t="s" s="1" r="J18">
         <v>21</v>
@@ -1508,10 +1487,10 @@
         <v>41</v>
       </c>
       <c t="s" s="1" r="N18">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c t="s" s="1" r="O18">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c s="1" r="P18"/>
       <c s="1" r="Q18"/>
@@ -1521,7 +1500,7 @@
     </row>
     <row r="19">
       <c t="s" s="1" r="A19">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c s="1" r="B19">
         <v>31</v>
@@ -1542,10 +1521,10 @@
         <v>6</v>
       </c>
       <c t="s" s="1" r="H19">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c t="s" s="1" r="I19">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c t="s" s="1" r="J19">
         <v>21</v>
@@ -1554,19 +1533,19 @@
         <v>42</v>
       </c>
       <c t="s" s="1" r="L19">
+        <v>110</v>
+      </c>
+      <c t="s" s="1" r="M19">
+        <v>111</v>
+      </c>
+      <c t="s" s="1" r="N19">
+        <v>95</v>
+      </c>
+      <c t="s" s="1" r="O19">
         <v>112</v>
       </c>
-      <c t="s" s="1" r="M19">
+      <c t="s" s="1" r="P19">
         <v>113</v>
-      </c>
-      <c t="s" s="1" r="N19">
-        <v>96</v>
-      </c>
-      <c t="s" s="1" r="O19">
-        <v>114</v>
-      </c>
-      <c t="s" s="1" r="P19">
-        <v>115</v>
       </c>
       <c s="1" r="Q19"/>
       <c s="1" r="R19"/>
@@ -1575,7 +1554,7 @@
     </row>
     <row r="20">
       <c t="s" s="1" r="A20">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c s="1" r="B20">
         <v>1</v>
@@ -1584,40 +1563,40 @@
         <v>29</v>
       </c>
       <c t="s" s="1" r="D20">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c t="s" s="1" r="E20">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c t="s" s="1" r="F20">
         <v>31</v>
       </c>
       <c t="s" s="1" r="G20">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c t="s" s="1" r="H20">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c t="s" s="1" r="I20">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c t="s" s="1" r="J20">
         <v>21</v>
       </c>
       <c t="s" s="1" r="K20">
+        <v>79</v>
+      </c>
+      <c t="s" s="1" r="L20">
         <v>80</v>
       </c>
-      <c t="s" s="1" r="L20">
+      <c t="s" s="1" r="M20">
         <v>81</v>
       </c>
-      <c t="s" s="1" r="M20">
+      <c t="s" s="1" r="N20">
         <v>82</v>
       </c>
-      <c t="s" s="1" r="N20">
-        <v>83</v>
-      </c>
       <c t="s" s="1" r="O20">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c s="1" r="P20"/>
       <c s="1" r="Q20"/>
@@ -1627,7 +1606,7 @@
     </row>
     <row r="21">
       <c t="s" s="1" r="A21">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c s="1" r="B21">
         <v>13</v>
@@ -1648,31 +1627,31 @@
         <v>6</v>
       </c>
       <c t="s" s="1" r="H21">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c t="s" s="1" r="I21">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c t="s" s="1" r="J21">
         <v>21</v>
       </c>
       <c t="s" s="1" r="K21">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c t="s" s="1" r="L21">
         <v>34</v>
       </c>
       <c t="s" s="1" r="M21">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c t="s" s="1" r="N21">
         <v>58</v>
       </c>
       <c t="s" s="1" r="O21">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c t="s" s="1" r="P21">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c s="1" r="Q21"/>
       <c s="1" r="R21"/>
@@ -1681,7 +1660,7 @@
     </row>
     <row r="22">
       <c t="s" s="1" r="A22">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c s="1" r="B22">
         <v>24</v>
@@ -1702,22 +1681,22 @@
         <v>13</v>
       </c>
       <c t="s" s="1" r="H22">
+        <v>121</v>
+      </c>
+      <c t="s" s="1" r="I22">
+        <v>122</v>
+      </c>
+      <c t="s" s="1" r="J22">
+        <v>21</v>
+      </c>
+      <c t="s" s="1" r="K22">
         <v>123</v>
       </c>
-      <c t="s" s="1" r="I22">
+      <c t="s" s="1" r="L22">
         <v>124</v>
       </c>
-      <c t="s" s="1" r="J22">
-        <v>21</v>
-      </c>
-      <c t="s" s="1" r="K22">
-        <v>125</v>
-      </c>
-      <c t="s" s="1" r="L22">
-        <v>126</v>
-      </c>
       <c t="s" s="1" r="M22">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c s="1" r="N22"/>
       <c s="1" r="O22"/>
@@ -1729,7 +1708,7 @@
     </row>
     <row r="23">
       <c t="s" s="1" r="A23">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c s="1" r="B23">
         <v>21</v>
@@ -1750,10 +1729,10 @@
         <v>6</v>
       </c>
       <c t="s" s="1" r="H23">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c t="s" s="1" r="I23">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c t="s" s="1" r="J23">
         <v>21</v>
@@ -1779,7 +1758,7 @@
     </row>
     <row r="24">
       <c t="s" s="1" r="A24">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c s="1" r="B24">
         <v>7</v>
@@ -1800,10 +1779,10 @@
         <v>2</v>
       </c>
       <c t="s" s="1" r="H24">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c t="s" s="1" r="I24">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c t="s" s="1" r="J24">
         <v>21</v>
@@ -1812,13 +1791,13 @@
         <v>33</v>
       </c>
       <c t="s" s="1" r="L24">
+        <v>129</v>
+      </c>
+      <c t="s" s="1" r="M24">
+        <v>130</v>
+      </c>
+      <c t="s" s="1" r="N24">
         <v>131</v>
-      </c>
-      <c t="s" s="1" r="M24">
-        <v>132</v>
-      </c>
-      <c t="s" s="1" r="N24">
-        <v>133</v>
       </c>
       <c s="1" r="O24"/>
       <c s="1" r="P24"/>
@@ -1829,7 +1808,7 @@
     </row>
     <row r="25">
       <c t="s" s="1" r="A25">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c s="1" r="B25">
         <v>23</v>
@@ -1850,10 +1829,10 @@
         <v>7</v>
       </c>
       <c t="s" s="1" r="H25">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c t="s" s="1" r="I25">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c t="s" s="1" r="J25">
         <v>21</v>
@@ -1862,7 +1841,7 @@
         <v>34</v>
       </c>
       <c t="s" s="1" r="L25">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c t="s" s="1" r="M25">
         <v>58</v>
@@ -1879,7 +1858,7 @@
     </row>
     <row r="26">
       <c t="s" s="1" r="A26">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c s="1" r="B26">
         <v>5</v>
@@ -1900,10 +1879,10 @@
         <v>1</v>
       </c>
       <c t="s" s="1" r="H26">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c t="s" s="1" r="I26">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c t="s" s="1" r="J26">
         <v>21</v>
@@ -1912,13 +1891,13 @@
         <v>42</v>
       </c>
       <c t="s" s="1" r="L26">
+        <v>95</v>
+      </c>
+      <c t="s" s="1" r="M26">
         <v>96</v>
       </c>
-      <c t="s" s="1" r="M26">
-        <v>97</v>
-      </c>
       <c t="s" s="1" r="N26">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c s="1" r="O26"/>
       <c s="1" r="P26"/>
@@ -1929,7 +1908,7 @@
     </row>
     <row r="27">
       <c t="s" s="1" r="A27">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c s="1" r="B27">
         <v>4</v>
@@ -1950,28 +1929,28 @@
         <v>1</v>
       </c>
       <c t="s" s="1" r="H27">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c t="s" s="1" r="I27">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c t="s" s="1" r="J27">
         <v>21</v>
       </c>
       <c t="s" s="1" r="K27">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c t="s" s="1" r="L27">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c t="s" s="1" r="M27">
         <v>58</v>
       </c>
       <c t="s" s="1" r="N27">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c t="s" s="1" r="O27">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c t="s" s="1" r="P27">
         <v>39</v>
@@ -1983,7 +1962,7 @@
     </row>
     <row r="28">
       <c t="s" s="1" r="A28">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c s="1" r="B28">
         <v>2</v>
@@ -2004,10 +1983,10 @@
         <v>1</v>
       </c>
       <c t="s" s="1" r="H28">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c t="s" s="1" r="I28">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c t="s" s="1" r="J28">
         <v>21</v>
@@ -2022,10 +2001,10 @@
         <v>41</v>
       </c>
       <c t="s" s="1" r="N28">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c t="s" s="1" r="O28">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c s="1" r="P28"/>
       <c s="1" r="Q28"/>
@@ -2035,7 +2014,7 @@
     </row>
     <row r="29">
       <c t="s" s="1" r="A29">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c s="1" r="B29">
         <v>1</v>
@@ -2044,40 +2023,40 @@
         <v>17</v>
       </c>
       <c t="s" s="1" r="D29">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c t="s" s="1" r="E29">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c t="s" s="1" r="F29">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c t="s" s="1" r="G29">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c t="s" s="1" r="H29">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c t="s" s="1" r="I29">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c t="s" s="1" r="J29">
         <v>21</v>
       </c>
       <c t="s" s="1" r="K29">
+        <v>79</v>
+      </c>
+      <c t="s" s="1" r="L29">
         <v>80</v>
       </c>
-      <c t="s" s="1" r="L29">
+      <c t="s" s="1" r="M29">
         <v>81</v>
       </c>
-      <c t="s" s="1" r="M29">
+      <c t="s" s="1" r="N29">
         <v>82</v>
       </c>
-      <c t="s" s="1" r="N29">
-        <v>83</v>
-      </c>
       <c t="s" s="1" r="O29">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c s="1" r="P29"/>
       <c s="1" r="Q29"/>
@@ -2087,7 +2066,7 @@
     </row>
     <row r="30">
       <c t="s" s="1" r="A30">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c s="1" r="B30">
         <v>28</v>
@@ -2099,7 +2078,7 @@
         <v>45</v>
       </c>
       <c t="s" s="1" r="E30">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c t="s" s="1" r="F30">
         <v>31</v>
@@ -2108,28 +2087,28 @@
         <v>10</v>
       </c>
       <c t="s" s="1" r="H30">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c t="s" s="1" r="I30">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c t="s" s="1" r="J30">
         <v>21</v>
       </c>
       <c t="s" s="1" r="K30">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c t="s" s="1" r="L30">
         <v>41</v>
       </c>
       <c t="s" s="1" r="M30">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c t="s" s="1" r="N30">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c t="s" s="1" r="O30">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c s="1" r="P30"/>
       <c s="1" r="Q30"/>
@@ -2138,9 +2117,7 @@
       <c s="1" r="T30"/>
     </row>
     <row r="31">
-      <c t="s" s="1" r="A31">
-        <v>153</v>
-      </c>
+      <c s="1" r="A31"/>
       <c s="1" r="B31">
         <v>25</v>
       </c>
@@ -2150,9 +2127,7 @@
       <c s="1" r="D31">
         <v>10</v>
       </c>
-      <c t="s" s="1" r="E31">
-        <v>18</v>
-      </c>
+      <c s="1" r="E31"/>
       <c s="1" r="F31">
         <v>10</v>
       </c>
@@ -2160,28 +2135,28 @@
         <v>4</v>
       </c>
       <c t="s" s="1" r="H31">
+        <v>151</v>
+      </c>
+      <c t="s" s="1" r="I31">
+        <v>148</v>
+      </c>
+      <c t="s" s="1" r="J31">
+        <v>21</v>
+      </c>
+      <c t="s" s="1" r="K31">
+        <v>152</v>
+      </c>
+      <c t="s" s="1" r="L31">
+        <v>153</v>
+      </c>
+      <c t="s" s="1" r="M31">
+        <v>112</v>
+      </c>
+      <c t="s" s="1" r="N31">
         <v>154</v>
       </c>
-      <c t="s" s="1" r="I31">
-        <v>150</v>
-      </c>
-      <c t="s" s="1" r="J31">
-        <v>21</v>
-      </c>
-      <c t="s" s="1" r="K31">
-        <v>155</v>
-      </c>
-      <c t="s" s="1" r="L31">
-        <v>156</v>
-      </c>
-      <c t="s" s="1" r="M31">
-        <v>114</v>
-      </c>
-      <c t="s" s="1" r="N31">
-        <v>157</v>
-      </c>
       <c t="s" s="1" r="O31">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c t="s" s="1" r="P31">
         <v>58</v>
@@ -2193,7 +2168,7 @@
     </row>
     <row r="32">
       <c t="s" s="1" r="A32">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c s="1" r="B32">
         <v>5</v>
@@ -2214,10 +2189,10 @@
         <v>5</v>
       </c>
       <c t="s" s="1" r="H32">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c t="s" s="1" r="I32">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c t="s" s="1" r="J32">
         <v>21</v>
@@ -2245,7 +2220,7 @@
     </row>
     <row r="33">
       <c t="s" s="1" r="A33">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c s="1" r="B33">
         <v>32</v>
@@ -2257,7 +2232,7 @@
         <v>36</v>
       </c>
       <c t="s" s="1" r="E33">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c t="s" s="1" r="F33">
         <v>31</v>
@@ -2266,28 +2241,28 @@
         <v>13</v>
       </c>
       <c t="s" s="1" r="H33">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c t="s" s="1" r="I33">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c t="s" s="1" r="J33">
         <v>21</v>
       </c>
       <c t="s" s="1" r="K33">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c t="s" s="1" r="L33">
         <v>41</v>
       </c>
       <c t="s" s="1" r="M33">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c t="s" s="1" r="N33">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c t="s" s="1" r="O33">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c s="1" r="P33"/>
       <c s="1" r="Q33"/>
@@ -2297,7 +2272,7 @@
     </row>
     <row r="34">
       <c t="s" s="1" r="A34">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c s="1" r="B34">
         <v>4</v>
@@ -2318,28 +2293,28 @@
         <v>1</v>
       </c>
       <c t="s" s="1" r="H34">
+        <v>161</v>
+      </c>
+      <c t="s" s="1" r="I34">
+        <v>159</v>
+      </c>
+      <c t="s" s="1" r="J34">
+        <v>21</v>
+      </c>
+      <c t="s" s="1" r="K34">
+        <v>162</v>
+      </c>
+      <c t="s" s="1" r="L34">
+        <v>163</v>
+      </c>
+      <c t="s" s="1" r="M34">
         <v>164</v>
       </c>
-      <c t="s" s="1" r="I34">
-        <v>162</v>
-      </c>
-      <c t="s" s="1" r="J34">
-        <v>21</v>
-      </c>
-      <c t="s" s="1" r="K34">
+      <c t="s" s="1" r="N34">
         <v>165</v>
       </c>
-      <c t="s" s="1" r="L34">
-        <v>166</v>
-      </c>
-      <c t="s" s="1" r="M34">
-        <v>167</v>
-      </c>
-      <c t="s" s="1" r="N34">
-        <v>168</v>
-      </c>
       <c t="s" s="1" r="O34">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c s="1" r="P34"/>
       <c s="1" r="Q34"/>
@@ -2349,7 +2324,7 @@
     </row>
     <row r="35">
       <c t="s" s="1" r="A35">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c s="1" r="B35">
         <v>2</v>
@@ -2368,10 +2343,10 @@
       </c>
       <c s="1" r="G35"/>
       <c t="s" s="1" r="H35">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c t="s" s="1" r="I35">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c t="s" s="1" r="J35">
         <v>21</v>
@@ -2386,10 +2361,10 @@
         <v>41</v>
       </c>
       <c t="s" s="1" r="N35">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c t="s" s="1" r="O35">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c s="1" r="P35"/>
       <c s="1" r="Q35"/>
@@ -2399,7 +2374,7 @@
     </row>
     <row r="36">
       <c t="s" s="1" r="A36">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c s="1" r="B36">
         <v>1</v>
@@ -2408,40 +2383,40 @@
         <v>29</v>
       </c>
       <c t="s" s="1" r="D36">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c t="s" s="1" r="E36">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c t="s" s="1" r="F36">
         <v>31</v>
       </c>
       <c t="s" s="1" r="G36">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c t="s" s="1" r="H36">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c t="s" s="1" r="I36">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c t="s" s="1" r="J36">
         <v>21</v>
       </c>
       <c t="s" s="1" r="K36">
+        <v>79</v>
+      </c>
+      <c t="s" s="1" r="L36">
         <v>80</v>
       </c>
-      <c t="s" s="1" r="L36">
+      <c t="s" s="1" r="M36">
         <v>81</v>
       </c>
-      <c t="s" s="1" r="M36">
+      <c t="s" s="1" r="N36">
         <v>82</v>
       </c>
-      <c t="s" s="1" r="N36">
-        <v>83</v>
-      </c>
       <c t="s" s="1" r="O36">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c s="1" r="P36"/>
       <c s="1" r="Q36"/>
@@ -2451,7 +2426,7 @@
     </row>
     <row r="37">
       <c t="s" s="1" r="A37">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c s="1" r="B37">
         <v>28</v>
@@ -2472,10 +2447,10 @@
         <v>10</v>
       </c>
       <c t="s" s="1" r="H37">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c t="s" s="1" r="I37">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c t="s" s="1" r="J37">
         <v>21</v>
@@ -2484,7 +2459,7 @@
         <v>34</v>
       </c>
       <c t="s" s="1" r="L37">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c t="s" s="1" r="M37">
         <v>58</v>
@@ -2501,7 +2476,7 @@
     </row>
     <row r="38">
       <c t="s" s="1" r="A38">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c s="1" r="B38">
         <v>27</v>
@@ -2522,28 +2497,28 @@
         <v>11</v>
       </c>
       <c t="s" s="1" r="H38">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c t="s" s="1" r="I38">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c t="s" s="1" r="J38">
         <v>21</v>
       </c>
       <c t="s" s="1" r="K38">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c t="s" s="1" r="L38">
         <v>41</v>
       </c>
       <c t="s" s="1" r="M38">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c t="s" s="1" r="N38">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c t="s" s="1" r="O38">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c s="1" r="P38"/>
       <c s="1" r="Q38"/>

</xml_diff>